<commit_message>
Upload a coule of misc files
</commit_message>
<xml_diff>
--- a/python/misc/diff_in_py2_and_py3.xlsx
+++ b/python/misc/diff_in_py2_and_py3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>python2</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>suppport star expressions：                           first, *middle, last = grades</t>
+  </si>
+  <si>
+    <t>anydbm , Queue , thread , StringIO.StringIO , urllib.open</t>
+  </si>
+  <si>
+    <t>dbm , queue , _thread , io.StringIO , urllib.request.urlopen</t>
   </si>
 </sst>
 </file>
@@ -33,11 +39,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,9 +73,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
+      <name val="WenQuanYi Micro Hei"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="WenQuanYi Micro Hei"/>
       <family val="0"/>
       <charset val="1"/>
@@ -116,7 +130,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,6 +145,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -150,16 +168,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -174,6 +192,14 @@
     <row r="2" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>